<commit_message>
updating lcoh code 8/5
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/raw/lcoh_policy_modeling_input.xlsx
+++ b/state_fact_sheets/data/raw/lcoh_policy_modeling_input.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanor/Documents/Industrial_Decarbonization/policy-team-workstream/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eleanor/Documents/Industrial_Decarbonization/Industrial-decarb/state_fact_sheets/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{098AAF34-C76B-574F-B032-A435ED48C8CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61C0BA9-7DDA-8F4A-A52E-AE927861D2BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30740" yWindow="-8660" windowWidth="36980" windowHeight="19700" xr2:uid="{15DD5EA5-1606-8E40-83C4-270FB523D3F5}"/>
+    <workbookView xWindow="18740" yWindow="2300" windowWidth="40960" windowHeight="24840" xr2:uid="{15DD5EA5-1606-8E40-83C4-270FB523D3F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,15 +62,6 @@
   </si>
   <si>
     <t>scenario_1_worst</t>
-  </si>
-  <si>
-    <t>Sappi Cloquet</t>
-  </si>
-  <si>
-    <t>Boise</t>
-  </si>
-  <si>
-    <t>Westrock</t>
   </si>
   <si>
     <t>AL CORN CLEAN FUEL</t>
@@ -173,6 +164,15 @@
   </si>
   <si>
     <t>scenario_4_best</t>
+  </si>
+  <si>
+    <t>SAPPI CLOQUET LLC</t>
+  </si>
+  <si>
+    <t>BOISE WHITE PAPER LLC</t>
+  </si>
+  <si>
+    <t>WestRock MN Corporation</t>
   </si>
 </sst>
 </file>
@@ -542,7 +542,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A170" sqref="A170:A172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -577,17 +577,17 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
+      <c r="A2" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="1">
         <v>322120</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>36</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -603,17 +603,17 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+      <c r="A3" t="s">
+        <v>44</v>
       </c>
       <c r="B3" s="1">
         <v>322120</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -629,17 +629,17 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
+      <c r="A4" t="s">
+        <v>45</v>
       </c>
       <c r="B4" s="1">
         <v>322130</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -656,16 +656,16 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="1">
         <v>325193</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -682,16 +682,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>325193</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -708,16 +708,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>325193</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -734,16 +734,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1">
         <v>325193</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -760,16 +760,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>325193</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -786,16 +786,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1">
         <v>325193</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -812,16 +812,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>325193</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -838,16 +838,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
         <v>325193</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -864,16 +864,16 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>325193</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -890,16 +890,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1">
         <v>325193</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -916,16 +916,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1">
         <v>325193</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -942,16 +942,16 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>325193</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -968,16 +968,16 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B17" s="1">
         <v>325193</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E17" t="s">
         <v>8</v>
@@ -994,16 +994,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B18" s="1">
         <v>325193</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
         <v>8</v>
@@ -1020,16 +1020,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B19" s="1">
         <v>325193</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1046,16 +1046,16 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B20" s="1">
         <v>325193</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1072,16 +1072,16 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1">
         <v>325193</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1098,16 +1098,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1">
         <v>311313</v>
       </c>
       <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
         <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>38</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1124,16 +1124,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" s="1">
         <v>311313</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
         <v>35</v>
-      </c>
-      <c r="D23" t="s">
-        <v>38</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1150,16 +1150,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B24" s="1">
         <v>311313</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
         <v>35</v>
-      </c>
-      <c r="D24" t="s">
-        <v>38</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1176,16 +1176,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B25" s="1">
         <v>311313</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" t="s">
         <v>35</v>
-      </c>
-      <c r="D25" t="s">
-        <v>38</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1201,20 +1201,20 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>9</v>
+      <c r="A26" t="s">
+        <v>43</v>
       </c>
       <c r="B26" s="1">
         <v>322120</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" t="s">
         <v>33</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>36</v>
-      </c>
-      <c r="E26" t="s">
-        <v>39</v>
       </c>
       <c r="F26" s="1">
         <v>1084084.824</v>
@@ -1227,20 +1227,20 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
-        <v>10</v>
+      <c r="A27" t="s">
+        <v>44</v>
       </c>
       <c r="B27" s="1">
         <v>322120</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" t="s">
         <v>33</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>36</v>
-      </c>
-      <c r="E27" t="s">
-        <v>39</v>
       </c>
       <c r="F27" s="1">
         <v>1162531.4480000001</v>
@@ -1253,20 +1253,20 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
-        <v>11</v>
+      <c r="A28" t="s">
+        <v>45</v>
       </c>
       <c r="B28" s="1">
         <v>322130</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" t="s">
         <v>33</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>36</v>
-      </c>
-      <c r="E28" t="s">
-        <v>39</v>
       </c>
       <c r="F28" s="1">
         <v>589310.43559999997</v>
@@ -1280,19 +1280,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B29" s="1">
         <v>325193</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F29" s="1">
         <v>1821134.0109999999</v>
@@ -1306,19 +1306,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B30" s="1">
         <v>325193</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F30" s="1">
         <v>1063717.1969999999</v>
@@ -1332,19 +1332,19 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B31" s="1">
         <v>325193</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F31" s="1">
         <v>691440.36399999994</v>
@@ -1358,19 +1358,19 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B32" s="1">
         <v>325193</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F32" s="1">
         <v>372115.65299999999</v>
@@ -1384,19 +1384,19 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B33" s="1">
         <v>325193</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E33" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F33" s="1">
         <v>753847.18819999998</v>
@@ -1410,19 +1410,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1">
         <v>325193</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F34" s="1">
         <v>1500382.8130000001</v>
@@ -1436,19 +1436,19 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B35" s="1">
         <v>325193</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F35" s="1">
         <v>820812.26249999995</v>
@@ -1462,19 +1462,19 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B36" s="1">
         <v>325193</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F36" s="1">
         <v>682097.81850000005</v>
@@ -1488,19 +1488,19 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B37" s="1">
         <v>325193</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E37" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F37" s="1">
         <v>1736549.622</v>
@@ -1514,19 +1514,19 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B38" s="1">
         <v>325193</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E38" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F38" s="1">
         <v>1877176.4650000001</v>
@@ -1540,19 +1540,19 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B39" s="1">
         <v>325193</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E39" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F39" s="1">
         <v>745072.3702</v>
@@ -1566,19 +1566,19 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B40" s="1">
         <v>325193</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E40" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F40" s="1">
         <v>767652.0612</v>
@@ -1592,19 +1592,19 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B41" s="1">
         <v>325193</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E41" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F41" s="1">
         <v>500958.41399999999</v>
@@ -1618,19 +1618,19 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1">
         <v>325193</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E42" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F42" s="1">
         <v>730691.23490000004</v>
@@ -1644,19 +1644,19 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B43" s="1">
         <v>325193</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D43" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F43" s="1">
         <v>723483.24730000005</v>
@@ -1670,19 +1670,19 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1">
         <v>325193</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F44" s="1">
         <v>767705.00730000006</v>
@@ -1696,19 +1696,19 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B45" s="1">
         <v>325193</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F45" s="1">
         <v>1774206.294</v>
@@ -1722,19 +1722,19 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B46" s="1">
         <v>311313</v>
       </c>
       <c r="C46" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" t="s">
         <v>35</v>
       </c>
-      <c r="D46" t="s">
-        <v>38</v>
-      </c>
       <c r="E46" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F46" s="1">
         <v>1321337.8659999999</v>
@@ -1748,19 +1748,19 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1">
         <v>311313</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s">
         <v>35</v>
       </c>
-      <c r="D47" t="s">
-        <v>38</v>
-      </c>
       <c r="E47" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F47" s="1">
         <v>1208755.851</v>
@@ -1774,19 +1774,19 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B48" s="1">
         <v>311313</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
         <v>35</v>
       </c>
-      <c r="D48" t="s">
-        <v>38</v>
-      </c>
       <c r="E48" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F48" s="1">
         <v>1315818.352</v>
@@ -1800,19 +1800,19 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1">
         <v>311313</v>
       </c>
       <c r="C49" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D49" t="s">
         <v>35</v>
       </c>
-      <c r="D49" t="s">
-        <v>38</v>
-      </c>
       <c r="E49" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F49" s="1">
         <v>2320500.6230000001</v>
@@ -1825,20 +1825,20 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="1" t="s">
-        <v>9</v>
+      <c r="A50" t="s">
+        <v>43</v>
       </c>
       <c r="B50" s="1">
         <v>322120</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" t="s">
         <v>33</v>
       </c>
-      <c r="D50" t="s">
-        <v>36</v>
-      </c>
       <c r="E50" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F50" s="1">
         <v>3826181.733</v>
@@ -1851,20 +1851,20 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="1" t="s">
-        <v>10</v>
+      <c r="A51" t="s">
+        <v>44</v>
       </c>
       <c r="B51" s="1">
         <v>322120</v>
       </c>
       <c r="C51" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D51" t="s">
         <v>33</v>
       </c>
-      <c r="D51" t="s">
-        <v>36</v>
-      </c>
       <c r="E51" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F51" s="1">
         <v>4103052.17</v>
@@ -1877,20 +1877,20 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="1" t="s">
-        <v>11</v>
+      <c r="A52" t="s">
+        <v>45</v>
       </c>
       <c r="B52" s="1">
         <v>322130</v>
       </c>
       <c r="C52" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D52" t="s">
         <v>33</v>
       </c>
-      <c r="D52" t="s">
-        <v>36</v>
-      </c>
       <c r="E52" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F52" s="1">
         <v>2079919.1850000001</v>
@@ -1904,19 +1904,19 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B53" s="1">
         <v>325193</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D53" t="s">
+        <v>34</v>
+      </c>
+      <c r="E53" t="s">
         <v>37</v>
-      </c>
-      <c r="E53" t="s">
-        <v>40</v>
       </c>
       <c r="F53" s="1">
         <v>6427531.8020000001</v>
@@ -1930,19 +1930,19 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B54" s="1">
         <v>325193</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D54" t="s">
+        <v>34</v>
+      </c>
+      <c r="E54" t="s">
         <v>37</v>
-      </c>
-      <c r="E54" t="s">
-        <v>40</v>
       </c>
       <c r="F54" s="1">
         <v>3754295.9909999999</v>
@@ -1956,19 +1956,19 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B55" s="1">
         <v>325193</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D55" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" t="s">
         <v>37</v>
-      </c>
-      <c r="E55" t="s">
-        <v>40</v>
       </c>
       <c r="F55" s="1">
         <v>2440377.7549999999</v>
@@ -1982,19 +1982,19 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B56" s="1">
         <v>325193</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D56" t="s">
+        <v>34</v>
+      </c>
+      <c r="E56" t="s">
         <v>37</v>
-      </c>
-      <c r="E56" t="s">
-        <v>40</v>
       </c>
       <c r="F56" s="1">
         <v>1313349.3640000001</v>
@@ -2008,19 +2008,19 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B57" s="1">
         <v>325193</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D57" t="s">
+        <v>34</v>
+      </c>
+      <c r="E57" t="s">
         <v>37</v>
-      </c>
-      <c r="E57" t="s">
-        <v>40</v>
       </c>
       <c r="F57" s="1">
         <v>2660637.1349999998</v>
@@ -2034,19 +2034,19 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B58" s="1">
         <v>325193</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D58" t="s">
+        <v>34</v>
+      </c>
+      <c r="E58" t="s">
         <v>37</v>
-      </c>
-      <c r="E58" t="s">
-        <v>40</v>
       </c>
       <c r="F58" s="1">
         <v>5295468.7510000002</v>
@@ -2060,19 +2060,19 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B59" s="1">
         <v>325193</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D59" t="s">
+        <v>34</v>
+      </c>
+      <c r="E59" t="s">
         <v>37</v>
-      </c>
-      <c r="E59" t="s">
-        <v>40</v>
       </c>
       <c r="F59" s="1">
         <v>2896984.4559999998</v>
@@ -2086,19 +2086,19 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B60" s="1">
         <v>325193</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s">
+        <v>34</v>
+      </c>
+      <c r="E60" t="s">
         <v>37</v>
-      </c>
-      <c r="E60" t="s">
-        <v>40</v>
       </c>
       <c r="F60" s="1">
         <v>2407404.0649999999</v>
@@ -2112,19 +2112,19 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B61" s="1">
         <v>325193</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D61" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" t="s">
         <v>37</v>
-      </c>
-      <c r="E61" t="s">
-        <v>40</v>
       </c>
       <c r="F61" s="1">
         <v>6128998.665</v>
@@ -2138,19 +2138,19 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B62" s="1">
         <v>325193</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D62" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" t="s">
         <v>37</v>
-      </c>
-      <c r="E62" t="s">
-        <v>40</v>
       </c>
       <c r="F62" s="1">
         <v>6625328.7010000004</v>
@@ -2164,19 +2164,19 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B63" s="1">
         <v>325193</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D63" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" t="s">
         <v>37</v>
-      </c>
-      <c r="E63" t="s">
-        <v>40</v>
       </c>
       <c r="F63" s="1">
         <v>2629667.1889999998</v>
@@ -2190,19 +2190,19 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B64" s="1">
         <v>325193</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D64" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" t="s">
         <v>37</v>
-      </c>
-      <c r="E64" t="s">
-        <v>40</v>
       </c>
       <c r="F64" s="1">
         <v>2709360.216</v>
@@ -2216,19 +2216,19 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B65" s="1">
         <v>325193</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D65" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" t="s">
         <v>37</v>
-      </c>
-      <c r="E65" t="s">
-        <v>40</v>
       </c>
       <c r="F65" s="1">
         <v>1768088.52</v>
@@ -2242,19 +2242,19 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B66" s="1">
         <v>325193</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D66" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" t="s">
         <v>37</v>
-      </c>
-      <c r="E66" t="s">
-        <v>40</v>
       </c>
       <c r="F66" s="1">
         <v>2578910.2409999999</v>
@@ -2268,19 +2268,19 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B67" s="1">
         <v>325193</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D67" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" t="s">
         <v>37</v>
-      </c>
-      <c r="E67" t="s">
-        <v>40</v>
       </c>
       <c r="F67" s="1">
         <v>2553470.2850000001</v>
@@ -2294,19 +2294,19 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B68" s="1">
         <v>325193</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D68" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" t="s">
         <v>37</v>
-      </c>
-      <c r="E68" t="s">
-        <v>40</v>
       </c>
       <c r="F68" s="1">
         <v>2709547.0839999998</v>
@@ -2320,19 +2320,19 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B69" s="1">
         <v>325193</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D69" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" t="s">
         <v>37</v>
-      </c>
-      <c r="E69" t="s">
-        <v>40</v>
       </c>
       <c r="F69" s="1">
         <v>6261904.5669999998</v>
@@ -2346,19 +2346,19 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B70" s="1">
         <v>311313</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D70" t="s">
         <v>35</v>
       </c>
-      <c r="D70" t="s">
-        <v>38</v>
-      </c>
       <c r="E70" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F70" s="1">
         <v>4663545.4079999998</v>
@@ -2372,19 +2372,19 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B71" s="1">
         <v>311313</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D71" t="s">
         <v>35</v>
       </c>
-      <c r="D71" t="s">
-        <v>38</v>
-      </c>
       <c r="E71" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F71" s="1">
         <v>4266197.1220000004</v>
@@ -2398,19 +2398,19 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B72" s="1">
         <v>311313</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" t="s">
         <v>35</v>
       </c>
-      <c r="D72" t="s">
-        <v>38</v>
-      </c>
       <c r="E72" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F72" s="1">
         <v>4644064.7709999997</v>
@@ -2424,19 +2424,19 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B73" s="1">
         <v>311313</v>
       </c>
       <c r="C73" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D73" t="s">
         <v>35</v>
       </c>
-      <c r="D73" t="s">
-        <v>38</v>
-      </c>
       <c r="E73" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F73" s="1">
         <v>8190002.199</v>
@@ -2449,20 +2449,20 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>9</v>
+      <c r="A74" t="s">
+        <v>43</v>
       </c>
       <c r="B74" s="1">
         <v>322120</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" t="s">
         <v>33</v>
       </c>
-      <c r="D74" t="s">
-        <v>36</v>
-      </c>
       <c r="E74" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F74" s="1">
         <v>1084084.824</v>
@@ -2475,20 +2475,20 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
-        <v>10</v>
+      <c r="A75" t="s">
+        <v>44</v>
       </c>
       <c r="B75" s="1">
         <v>322120</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" t="s">
         <v>33</v>
       </c>
-      <c r="D75" t="s">
-        <v>36</v>
-      </c>
       <c r="E75" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F75" s="1">
         <v>1162531.4480000001</v>
@@ -2501,20 +2501,20 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>11</v>
+      <c r="A76" t="s">
+        <v>45</v>
       </c>
       <c r="B76" s="1">
         <v>322130</v>
       </c>
       <c r="C76" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" t="s">
         <v>33</v>
       </c>
-      <c r="D76" t="s">
-        <v>36</v>
-      </c>
       <c r="E76" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F76" s="1">
         <v>589310.43559999997</v>
@@ -2528,19 +2528,19 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B77" s="1">
         <v>325193</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D77" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E77" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F77" s="1">
         <v>1821134.0109999999</v>
@@ -2554,19 +2554,19 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B78" s="1">
         <v>325193</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D78" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E78" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F78" s="1">
         <v>1063717.1969999999</v>
@@ -2580,19 +2580,19 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B79" s="1">
         <v>325193</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D79" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E79" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F79" s="1">
         <v>691440.36399999994</v>
@@ -2606,19 +2606,19 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B80" s="1">
         <v>325193</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D80" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E80" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F80" s="1">
         <v>372115.65299999999</v>
@@ -2632,19 +2632,19 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B81" s="1">
         <v>325193</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D81" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E81" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F81" s="1">
         <v>753847.18819999998</v>
@@ -2658,19 +2658,19 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B82" s="1">
         <v>325193</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D82" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E82" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F82" s="1">
         <v>1500382.8130000001</v>
@@ -2684,19 +2684,19 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B83" s="1">
         <v>325193</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D83" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E83" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F83" s="1">
         <v>820812.26249999995</v>
@@ -2710,19 +2710,19 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B84" s="1">
         <v>325193</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D84" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E84" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F84" s="1">
         <v>682097.81850000005</v>
@@ -2736,19 +2736,19 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B85" s="1">
         <v>325193</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D85" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E85" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F85" s="1">
         <v>1736549.622</v>
@@ -2762,19 +2762,19 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B86" s="1">
         <v>325193</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D86" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E86" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F86" s="1">
         <v>1877176.4650000001</v>
@@ -2788,19 +2788,19 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B87" s="1">
         <v>325193</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D87" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E87" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F87" s="1">
         <v>745072.3702</v>
@@ -2814,19 +2814,19 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B88" s="1">
         <v>325193</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D88" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E88" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F88" s="1">
         <v>767652.0612</v>
@@ -2840,19 +2840,19 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B89" s="1">
         <v>325193</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D89" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E89" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F89" s="1">
         <v>500958.41399999999</v>
@@ -2866,19 +2866,19 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B90" s="1">
         <v>325193</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D90" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E90" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F90" s="1">
         <v>730691.23490000004</v>
@@ -2892,19 +2892,19 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B91" s="1">
         <v>325193</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D91" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E91" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F91" s="1">
         <v>723483.24730000005</v>
@@ -2918,19 +2918,19 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B92" s="1">
         <v>325193</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D92" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E92" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F92" s="1">
         <v>767705.00730000006</v>
@@ -2944,19 +2944,19 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B93" s="1">
         <v>325193</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D93" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E93" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F93" s="1">
         <v>1774206.294</v>
@@ -2970,19 +2970,19 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B94" s="1">
         <v>311313</v>
       </c>
       <c r="C94" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D94" t="s">
         <v>35</v>
       </c>
-      <c r="D94" t="s">
+      <c r="E94" t="s">
         <v>38</v>
-      </c>
-      <c r="E94" t="s">
-        <v>41</v>
       </c>
       <c r="F94" s="1">
         <v>1321337.8659999999</v>
@@ -2996,19 +2996,19 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B95" s="1">
         <v>311313</v>
       </c>
       <c r="C95" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D95" t="s">
         <v>35</v>
       </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>38</v>
-      </c>
-      <c r="E95" t="s">
-        <v>41</v>
       </c>
       <c r="F95" s="1">
         <v>1208755.851</v>
@@ -3022,19 +3022,19 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B96" s="1">
         <v>311313</v>
       </c>
       <c r="C96" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D96" t="s">
         <v>35</v>
       </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>38</v>
-      </c>
-      <c r="E96" t="s">
-        <v>41</v>
       </c>
       <c r="F96" s="1">
         <v>1315818.352</v>
@@ -3048,19 +3048,19 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B97" s="1">
         <v>311313</v>
       </c>
       <c r="C97" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D97" t="s">
         <v>35</v>
       </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>38</v>
-      </c>
-      <c r="E97" t="s">
-        <v>41</v>
       </c>
       <c r="F97" s="1">
         <v>2320500.6230000001</v>
@@ -3073,20 +3073,20 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="1" t="s">
-        <v>9</v>
+      <c r="A98" t="s">
+        <v>43</v>
       </c>
       <c r="B98" s="1">
         <v>322120</v>
       </c>
       <c r="C98" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D98" t="s">
         <v>33</v>
       </c>
-      <c r="D98" t="s">
-        <v>36</v>
-      </c>
       <c r="E98" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F98" s="1">
         <v>63769695.549999997</v>
@@ -3099,20 +3099,20 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="1" t="s">
-        <v>10</v>
+      <c r="A99" t="s">
+        <v>44</v>
       </c>
       <c r="B99" s="1">
         <v>322120</v>
       </c>
       <c r="C99" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D99" t="s">
         <v>33</v>
       </c>
-      <c r="D99" t="s">
-        <v>36</v>
-      </c>
       <c r="E99" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F99" s="1">
         <v>68384202.840000004</v>
@@ -3125,20 +3125,20 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="1" t="s">
-        <v>11</v>
+      <c r="A100" t="s">
+        <v>45</v>
       </c>
       <c r="B100" s="1">
         <v>322130</v>
       </c>
       <c r="C100" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D100" t="s">
         <v>33</v>
       </c>
-      <c r="D100" t="s">
-        <v>36</v>
-      </c>
       <c r="E100" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F100" s="1">
         <v>34665319.740000002</v>
@@ -3152,19 +3152,19 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B101" s="1">
         <v>325193</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D101" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E101" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F101" s="1">
         <v>107125530</v>
@@ -3178,19 +3178,19 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B102" s="1">
         <v>325193</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D102" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E102" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F102" s="1">
         <v>62571599.850000001</v>
@@ -3204,19 +3204,19 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B103" s="1">
         <v>325193</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D103" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E103" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F103" s="1">
         <v>40672962.590000004</v>
@@ -3230,19 +3230,19 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B104" s="1">
         <v>325193</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D104" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E104" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F104" s="1">
         <v>21889156.059999999</v>
@@ -3256,19 +3256,19 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B105" s="1">
         <v>325193</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D105" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E105" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F105" s="1">
         <v>44343952.25</v>
@@ -3282,19 +3282,19 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B106" s="1">
         <v>325193</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D106" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E106" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F106" s="1">
         <v>88257812.519999996</v>
@@ -3308,19 +3308,19 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B107" s="1">
         <v>325193</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D107" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E107" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F107" s="1">
         <v>48283074.259999998</v>
@@ -3334,19 +3334,19 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B108" s="1">
         <v>325193</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D108" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E108" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F108" s="1">
         <v>40123401.090000004</v>
@@ -3360,19 +3360,19 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B109" s="1">
         <v>325193</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D109" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E109" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F109" s="1">
         <v>102149977.7</v>
@@ -3386,19 +3386,19 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B110" s="1">
         <v>325193</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D110" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E110" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F110" s="1">
         <v>110422145</v>
@@ -3412,19 +3412,19 @@
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B111" s="1">
         <v>325193</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D111" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E111" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F111" s="1">
         <v>43827786.479999997</v>
@@ -3438,19 +3438,19 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B112" s="1">
         <v>325193</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D112" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E112" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F112" s="1">
         <v>45156003.600000001</v>
@@ -3464,19 +3464,19 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B113" s="1">
         <v>325193</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D113" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E113" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F113" s="1">
         <v>29468142</v>
@@ -3490,19 +3490,19 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B114" s="1">
         <v>325193</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D114" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E114" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F114" s="1">
         <v>42981837.350000001</v>
@@ -3516,19 +3516,19 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B115" s="1">
         <v>325193</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D115" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E115" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F115" s="1">
         <v>42557838.079999998</v>
@@ -3542,19 +3542,19 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B116" s="1">
         <v>325193</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D116" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E116" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F116" s="1">
         <v>45159118.07</v>
@@ -3568,19 +3568,19 @@
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B117" s="1">
         <v>325193</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D117" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E117" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F117" s="1">
         <v>104365076.09999999</v>
@@ -3594,19 +3594,19 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B118" s="1">
         <v>311313</v>
       </c>
       <c r="C118" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D118" t="s">
         <v>35</v>
       </c>
-      <c r="D118" t="s">
-        <v>38</v>
-      </c>
       <c r="E118" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F118" s="1">
         <v>77725756.799999997</v>
@@ -3620,19 +3620,19 @@
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B119" s="1">
         <v>311313</v>
       </c>
       <c r="C119" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D119" t="s">
         <v>35</v>
       </c>
-      <c r="D119" t="s">
-        <v>38</v>
-      </c>
       <c r="E119" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F119" s="1">
         <v>71103285.359999999</v>
@@ -3646,19 +3646,19 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B120" s="1">
         <v>311313</v>
       </c>
       <c r="C120" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D120" t="s">
         <v>35</v>
       </c>
-      <c r="D120" t="s">
-        <v>38</v>
-      </c>
       <c r="E120" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F120" s="1">
         <v>77401079.519999996</v>
@@ -3672,19 +3672,19 @@
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B121" s="1">
         <v>311313</v>
       </c>
       <c r="C121" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D121" t="s">
         <v>35</v>
       </c>
-      <c r="D121" t="s">
-        <v>38</v>
-      </c>
       <c r="E121" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F121" s="1">
         <v>136500036.69999999</v>
@@ -3697,20 +3697,20 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" s="1" t="s">
-        <v>9</v>
+      <c r="A122" t="s">
+        <v>43</v>
       </c>
       <c r="B122" s="1">
         <v>322120</v>
       </c>
       <c r="C122" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D122" t="s">
         <v>33</v>
       </c>
-      <c r="D122" t="s">
-        <v>36</v>
-      </c>
       <c r="E122" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F122" s="1">
         <v>19130908.670000002</v>
@@ -3723,20 +3723,20 @@
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A123" s="1" t="s">
-        <v>10</v>
+      <c r="A123" t="s">
+        <v>44</v>
       </c>
       <c r="B123" s="1">
         <v>322120</v>
       </c>
       <c r="C123" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D123" t="s">
         <v>33</v>
       </c>
-      <c r="D123" t="s">
-        <v>36</v>
-      </c>
       <c r="E123" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F123" s="1">
         <v>20515260.850000001</v>
@@ -3749,20 +3749,20 @@
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A124" s="1" t="s">
-        <v>11</v>
+      <c r="A124" t="s">
+        <v>45</v>
       </c>
       <c r="B124" s="1">
         <v>322130</v>
       </c>
       <c r="C124" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D124" t="s">
         <v>33</v>
       </c>
-      <c r="D124" t="s">
-        <v>36</v>
-      </c>
       <c r="E124" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F124" s="1">
         <v>10399595.92</v>
@@ -3776,19 +3776,19 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B125" s="1">
         <v>325193</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D125" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E125" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F125" s="1">
         <v>32137659.010000002</v>
@@ -3802,19 +3802,19 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B126" s="1">
         <v>325193</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D126" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E126" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F126" s="1">
         <v>18771479.949999999</v>
@@ -3828,19 +3828,19 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B127" s="1">
         <v>325193</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D127" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E127" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F127" s="1">
         <v>12201888.779999999</v>
@@ -3854,19 +3854,19 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B128" s="1">
         <v>325193</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D128" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E128" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F128" s="1">
         <v>6566746.818</v>
@@ -3880,19 +3880,19 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B129" s="1">
         <v>325193</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D129" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E129" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F129" s="1">
         <v>13303185.67</v>
@@ -3906,19 +3906,19 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B130" s="1">
         <v>325193</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D130" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E130" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F130" s="1">
         <v>26477343.760000002</v>
@@ -3932,19 +3932,19 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B131" s="1">
         <v>325193</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D131" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E131" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F131" s="1">
         <v>14484922.279999999</v>
@@ -3958,19 +3958,19 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B132" s="1">
         <v>325193</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D132" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E132" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F132" s="1">
         <v>12037020.33</v>
@@ -3984,19 +3984,19 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B133" s="1">
         <v>325193</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D133" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E133" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F133" s="1">
         <v>30644993.32</v>
@@ -4010,19 +4010,19 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B134" s="1">
         <v>325193</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D134" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E134" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F134" s="1">
         <v>33126643.5</v>
@@ -4036,19 +4036,19 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B135" s="1">
         <v>325193</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D135" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E135" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F135" s="1">
         <v>13148335.949999999</v>
@@ -4062,19 +4062,19 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B136" s="1">
         <v>325193</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D136" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E136" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F136" s="1">
         <v>13546801.08</v>
@@ -4088,19 +4088,19 @@
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B137" s="1">
         <v>325193</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D137" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E137" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F137" s="1">
         <v>8840442.6009999998</v>
@@ -4114,19 +4114,19 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B138" s="1">
         <v>325193</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D138" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E138" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F138" s="1">
         <v>12894551.199999999</v>
@@ -4140,19 +4140,19 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B139" s="1">
         <v>325193</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D139" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E139" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F139" s="1">
         <v>12767351.42</v>
@@ -4166,19 +4166,19 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B140" s="1">
         <v>325193</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D140" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E140" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F140" s="1">
         <v>13547735.42</v>
@@ -4192,19 +4192,19 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B141" s="1">
         <v>325193</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D141" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E141" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F141" s="1">
         <v>31309522.829999998</v>
@@ -4218,19 +4218,19 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B142" s="1">
         <v>311313</v>
       </c>
       <c r="C142" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D142" t="s">
         <v>35</v>
       </c>
-      <c r="D142" t="s">
-        <v>38</v>
-      </c>
       <c r="E142" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F142" s="1">
         <v>23317727.039999999</v>
@@ -4244,19 +4244,19 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B143" s="1">
         <v>311313</v>
       </c>
       <c r="C143" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D143" t="s">
         <v>35</v>
       </c>
-      <c r="D143" t="s">
-        <v>38</v>
-      </c>
       <c r="E143" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F143" s="1">
         <v>21330985.609999999</v>
@@ -4270,19 +4270,19 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B144" s="1">
         <v>311313</v>
       </c>
       <c r="C144" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D144" t="s">
         <v>35</v>
       </c>
-      <c r="D144" t="s">
-        <v>38</v>
-      </c>
       <c r="E144" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F144" s="1">
         <v>23220323.859999999</v>
@@ -4296,19 +4296,19 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B145" s="1">
         <v>311313</v>
       </c>
       <c r="C145" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D145" t="s">
         <v>35</v>
       </c>
-      <c r="D145" t="s">
-        <v>38</v>
-      </c>
       <c r="E145" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F145" s="1">
         <v>40950011</v>
@@ -4321,20 +4321,20 @@
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A146" s="1" t="s">
-        <v>9</v>
+      <c r="A146" t="s">
+        <v>43</v>
       </c>
       <c r="B146" s="1">
         <v>322120</v>
       </c>
       <c r="C146" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D146" t="s">
         <v>33</v>
       </c>
-      <c r="D146" t="s">
-        <v>36</v>
-      </c>
       <c r="E146" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F146" s="1">
         <v>63769695.549999997</v>
@@ -4347,20 +4347,20 @@
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A147" s="1" t="s">
-        <v>10</v>
+      <c r="A147" t="s">
+        <v>44</v>
       </c>
       <c r="B147" s="1">
         <v>322120</v>
       </c>
       <c r="C147" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D147" t="s">
         <v>33</v>
       </c>
-      <c r="D147" t="s">
-        <v>36</v>
-      </c>
       <c r="E147" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F147" s="1">
         <v>68384202.840000004</v>
@@ -4373,20 +4373,20 @@
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A148" s="1" t="s">
-        <v>11</v>
+      <c r="A148" t="s">
+        <v>45</v>
       </c>
       <c r="B148" s="1">
         <v>322130</v>
       </c>
       <c r="C148" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D148" t="s">
         <v>33</v>
       </c>
-      <c r="D148" t="s">
-        <v>36</v>
-      </c>
       <c r="E148" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F148" s="1">
         <v>34665319.740000002</v>
@@ -4400,19 +4400,19 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B149" s="1">
         <v>325193</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D149" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E149" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F149" s="1">
         <v>107125530</v>
@@ -4426,19 +4426,19 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B150" s="1">
         <v>325193</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D150" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E150" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F150" s="1">
         <v>62571599.850000001</v>
@@ -4452,19 +4452,19 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B151" s="1">
         <v>325193</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D151" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E151" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F151" s="1">
         <v>40672962.590000004</v>
@@ -4478,19 +4478,19 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B152" s="1">
         <v>325193</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D152" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E152" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F152" s="1">
         <v>21889156.059999999</v>
@@ -4504,19 +4504,19 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B153" s="1">
         <v>325193</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D153" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E153" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F153" s="1">
         <v>44343952.25</v>
@@ -4530,19 +4530,19 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B154" s="1">
         <v>325193</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D154" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E154" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F154" s="1">
         <v>88257812.519999996</v>
@@ -4556,19 +4556,19 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B155" s="1">
         <v>325193</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D155" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E155" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F155" s="1">
         <v>48283074.259999998</v>
@@ -4582,19 +4582,19 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B156" s="1">
         <v>325193</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D156" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E156" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F156" s="1">
         <v>40123401.090000004</v>
@@ -4608,19 +4608,19 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B157" s="1">
         <v>325193</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D157" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E157" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F157" s="1">
         <v>102149977.7</v>
@@ -4634,19 +4634,19 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B158" s="1">
         <v>325193</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D158" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E158" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F158" s="1">
         <v>110422145</v>
@@ -4660,19 +4660,19 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B159" s="1">
         <v>325193</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D159" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E159" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F159" s="1">
         <v>43827786.479999997</v>
@@ -4686,19 +4686,19 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B160" s="1">
         <v>325193</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D160" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E160" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F160" s="1">
         <v>45156003.600000001</v>
@@ -4712,19 +4712,19 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B161" s="1">
         <v>325193</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D161" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E161" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F161" s="1">
         <v>29468142</v>
@@ -4738,19 +4738,19 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B162" s="1">
         <v>325193</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D162" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E162" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F162" s="1">
         <v>42981837.350000001</v>
@@ -4764,19 +4764,19 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B163" s="1">
         <v>325193</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D163" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E163" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F163" s="1">
         <v>42557838.079999998</v>
@@ -4790,19 +4790,19 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B164" s="1">
         <v>325193</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D164" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E164" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F164" s="1">
         <v>45159118.07</v>
@@ -4816,19 +4816,19 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B165" s="1">
         <v>325193</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D165" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E165" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F165" s="1">
         <v>104365076.09999999</v>
@@ -4842,19 +4842,19 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B166" s="1">
         <v>311313</v>
       </c>
       <c r="C166" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D166" t="s">
         <v>35</v>
       </c>
-      <c r="D166" t="s">
-        <v>38</v>
-      </c>
       <c r="E166" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F166" s="1">
         <v>77725756.799999997</v>
@@ -4868,19 +4868,19 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B167" s="1">
         <v>311313</v>
       </c>
       <c r="C167" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D167" t="s">
         <v>35</v>
       </c>
-      <c r="D167" t="s">
-        <v>38</v>
-      </c>
       <c r="E167" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F167" s="1">
         <v>71103285.359999999</v>
@@ -4894,19 +4894,19 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B168" s="1">
         <v>311313</v>
       </c>
       <c r="C168" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D168" t="s">
         <v>35</v>
       </c>
-      <c r="D168" t="s">
-        <v>38</v>
-      </c>
       <c r="E168" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F168" s="1">
         <v>77401079.519999996</v>
@@ -4920,19 +4920,19 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B169" s="1">
         <v>311313</v>
       </c>
       <c r="C169" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D169" t="s">
         <v>35</v>
       </c>
-      <c r="D169" t="s">
-        <v>38</v>
-      </c>
       <c r="E169" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F169" s="1">
         <v>136500036.69999999</v>
@@ -4945,20 +4945,20 @@
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A170" s="1" t="s">
-        <v>9</v>
+      <c r="A170" t="s">
+        <v>43</v>
       </c>
       <c r="B170" s="1">
         <v>322120</v>
       </c>
       <c r="C170" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D170" t="s">
         <v>33</v>
       </c>
-      <c r="D170" t="s">
-        <v>36</v>
-      </c>
       <c r="E170" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F170" s="1">
         <v>19130908.670000002</v>
@@ -4971,20 +4971,20 @@
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A171" s="1" t="s">
-        <v>10</v>
+      <c r="A171" t="s">
+        <v>44</v>
       </c>
       <c r="B171" s="1">
         <v>322120</v>
       </c>
       <c r="C171" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D171" t="s">
         <v>33</v>
       </c>
-      <c r="D171" t="s">
-        <v>36</v>
-      </c>
       <c r="E171" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F171" s="1">
         <v>20515260.850000001</v>
@@ -4997,20 +4997,20 @@
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A172" s="1" t="s">
-        <v>11</v>
+      <c r="A172" t="s">
+        <v>45</v>
       </c>
       <c r="B172" s="1">
         <v>322130</v>
       </c>
       <c r="C172" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D172" t="s">
         <v>33</v>
       </c>
-      <c r="D172" t="s">
-        <v>36</v>
-      </c>
       <c r="E172" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F172" s="1">
         <v>10399595.92</v>
@@ -5024,19 +5024,19 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B173" s="1">
         <v>325193</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D173" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E173" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F173" s="1">
         <v>32137659.010000002</v>
@@ -5050,19 +5050,19 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B174" s="1">
         <v>325193</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D174" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E174" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F174" s="1">
         <v>18771479.949999999</v>
@@ -5076,19 +5076,19 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B175" s="1">
         <v>325193</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D175" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E175" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F175" s="1">
         <v>12201888.779999999</v>
@@ -5102,19 +5102,19 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B176" s="1">
         <v>325193</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D176" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E176" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F176" s="1">
         <v>6566746.818</v>
@@ -5128,19 +5128,19 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B177" s="1">
         <v>325193</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D177" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E177" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F177" s="1">
         <v>13303185.67</v>
@@ -5154,19 +5154,19 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B178" s="1">
         <v>325193</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D178" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E178" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F178" s="1">
         <v>26477343.760000002</v>
@@ -5180,19 +5180,19 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B179" s="1">
         <v>325193</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D179" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E179" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F179" s="1">
         <v>14484922.279999999</v>
@@ -5206,19 +5206,19 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B180" s="1">
         <v>325193</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D180" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E180" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F180" s="1">
         <v>12037020.33</v>
@@ -5232,19 +5232,19 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B181" s="1">
         <v>325193</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D181" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E181" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F181" s="1">
         <v>30644993.32</v>
@@ -5258,19 +5258,19 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B182" s="1">
         <v>325193</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D182" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E182" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F182" s="1">
         <v>33126643.5</v>
@@ -5284,19 +5284,19 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B183" s="1">
         <v>325193</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D183" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E183" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F183" s="1">
         <v>13148335.949999999</v>
@@ -5310,19 +5310,19 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B184" s="1">
         <v>325193</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D184" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E184" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F184" s="1">
         <v>13546801.08</v>
@@ -5336,19 +5336,19 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B185" s="1">
         <v>325193</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D185" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E185" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F185" s="1">
         <v>8840442.6009999998</v>
@@ -5362,19 +5362,19 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B186" s="1">
         <v>325193</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D186" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E186" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F186" s="1">
         <v>12894551.199999999</v>
@@ -5388,19 +5388,19 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B187" s="1">
         <v>325193</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D187" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E187" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F187" s="1">
         <v>12767351.42</v>
@@ -5414,19 +5414,19 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B188" s="1">
         <v>325193</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D188" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E188" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F188" s="1">
         <v>13547735.42</v>
@@ -5440,19 +5440,19 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B189" s="1">
         <v>325193</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D189" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E189" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F189" s="1">
         <v>31309522.829999998</v>
@@ -5466,19 +5466,19 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B190" s="1">
         <v>311313</v>
       </c>
       <c r="C190" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D190" t="s">
         <v>35</v>
       </c>
-      <c r="D190" t="s">
-        <v>38</v>
-      </c>
       <c r="E190" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F190" s="1">
         <v>23317727.039999999</v>
@@ -5492,19 +5492,19 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B191" s="1">
         <v>311313</v>
       </c>
       <c r="C191" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D191" t="s">
         <v>35</v>
       </c>
-      <c r="D191" t="s">
-        <v>38</v>
-      </c>
       <c r="E191" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F191" s="1">
         <v>21330985.609999999</v>
@@ -5518,19 +5518,19 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B192" s="1">
         <v>311313</v>
       </c>
       <c r="C192" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D192" t="s">
         <v>35</v>
       </c>
-      <c r="D192" t="s">
-        <v>38</v>
-      </c>
       <c r="E192" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F192" s="1">
         <v>23220323.859999999</v>
@@ -5544,19 +5544,19 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B193" s="1">
         <v>311313</v>
       </c>
       <c r="C193" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D193" t="s">
         <v>35</v>
       </c>
-      <c r="D193" t="s">
-        <v>38</v>
-      </c>
       <c r="E193" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F193" s="1">
         <v>40950011</v>

</xml_diff>